<commit_message>
file upload + algo
</commit_message>
<xml_diff>
--- a/specifications/Suivi garde Louise et Joséphine.xlsx
+++ b/specifications/Suivi garde Louise et Joséphine.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t>Horodateur</t>
   </si>
@@ -279,6 +279,68 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>43343.95301059028</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.32291666666424135</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>43343.953370034724</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.7083333333357587</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>43346.79166195602</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.38541666666424135</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>43346.79189278935</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.7083333333357587</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Mise en forme des données
</commit_message>
<xml_diff>
--- a/specifications/Suivi garde Louise et Joséphine.xlsx
+++ b/specifications/Suivi garde Louise et Joséphine.xlsx
@@ -1,18 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\Projets\calcul-assmat\specifications\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{17E6B0EA-B67A-4B2C-ACDD-77DD31CFD489}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Réponses au formulaire 1" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Feuille 1" sheetId="2" r:id="rId4"/>
+    <sheet name="Réponses au formulaire 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuille 1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="16">
   <si>
     <t>Horodateur</t>
   </si>
@@ -59,87 +68,383 @@
     <t>AR école X2</t>
   </si>
   <si>
-    <t>Autre (indiquer le kilométrage dans le champ suivant)</t>
+    <t>Déjeuner, Goûter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="19" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="19" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="14" width="21.57"/>
+    <col min="1" max="14" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -165,12 +470,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43343.92923055556</v>
+        <v>43343.929230555557</v>
       </c>
       <c r="B2" s="2">
-        <v>43339.0</v>
+        <v>43339</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>8</v>
@@ -182,12 +487,12 @@
         <v>0.32291666666424135</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43343.92957425926</v>
+        <v>43343.929574259259</v>
       </c>
       <c r="B3" s="2">
-        <v>43339.0</v>
+        <v>43339</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
@@ -196,18 +501,18 @@
         <v>11</v>
       </c>
       <c r="E3" s="4">
-        <v>0.7083333333357587</v>
+        <v>0.70833333333575865</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>43343.93097717593</v>
+        <v>43343.930977175929</v>
       </c>
       <c r="B4" s="2">
-        <v>43343.0</v>
+        <v>43343</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
@@ -219,12 +524,12 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43343.93125337963</v>
+        <v>43343.931253379633</v>
       </c>
       <c r="B5" s="2">
-        <v>43343.0</v>
+        <v>43343</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
@@ -242,12 +547,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43343.931597523144</v>
       </c>
       <c r="B6" s="2">
-        <v>43342.0</v>
+        <v>43342</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>8</v>
@@ -259,12 +564,12 @@
         <v>0.32291666666424135</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43343.93181945602</v>
+        <v>43343.931819456018</v>
       </c>
       <c r="B7" s="2">
-        <v>43342.0</v>
+        <v>43342</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
@@ -282,23 +587,23 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43343.95301059028</v>
+        <v>43346.79166195602</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="4">
-        <v>0.32291666666424135</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>0.38541666666424135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43343.953370034724</v>
+        <v>43346.791892789348</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
@@ -307,49 +612,55 @@
         <v>11</v>
       </c>
       <c r="E9" s="4">
-        <v>0.7083333333357587</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>0.70833333333575865</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43346.79166195602</v>
+        <v>43347.328665138892</v>
+      </c>
+      <c r="B10" s="2">
+        <v>43347</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="4">
-        <v>0.38541666666424135</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>0.32291666666424135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43346.79189278935</v>
+        <v>43347.794715173615</v>
+      </c>
+      <c r="B11" s="2">
+        <v>43347</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="4">
-        <v>0.7083333333357587</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>0.77083333333575865</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43347.32866513889</v>
+        <v>43349.921830497682</v>
       </c>
       <c r="B12" s="2">
-        <v>43347.0</v>
+        <v>43349</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
@@ -360,85 +671,146 @@
       <c r="E12" s="4">
         <v>0.32291666666424135</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13">
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>43347.794715173615</v>
+        <v>43349.922125462967</v>
       </c>
       <c r="B13" s="2">
-        <v>43347.0</v>
+        <v>43349</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="4">
-        <v>0.7708333333357587</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>13</v>
+        <v>0.72916666666424135</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>43349.92183049768</v>
+        <v>43350.783449976851</v>
       </c>
       <c r="B14" s="2">
-        <v>43349.0</v>
+        <v>43350</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="4">
-        <v>0.32291666666424135</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>43349.92212546297</v>
-      </c>
-      <c r="B15" s="2">
-        <v>43349.0</v>
+        <v>43350.783746875</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="4">
-        <v>0.7291666666642413</v>
+        <v>0.76041666666424135</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43353.883479074073</v>
+      </c>
+      <c r="B16" s="2">
+        <v>43353</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.32291666666424135</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43353.883786770835</v>
+      </c>
+      <c r="B17" s="2">
+        <v>43353</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.71875</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43353.89663181713</v>
+      </c>
+      <c r="B18" s="2">
+        <v>43322</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.33333333333575865</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="3">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>